<commit_message>
Teams.json and subs format
</commit_message>
<xml_diff>
--- a/data_files/MegaContest.xlsx
+++ b/data_files/MegaContest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rmanchanda/Desktop/HA/Fantasy/data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46D2A16-9C7A-8248-990A-08B047CF9A71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C4BD6E-CBFE-5444-911E-B33DCFA56142}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form responses 1" sheetId="1" r:id="rId1"/>
@@ -354,7 +354,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="171">
   <si>
     <t>Timestamp</t>
   </si>
@@ -425,9 +425,6 @@
     <t>Shubman Gill</t>
   </si>
   <si>
-    <t>Ashwin</t>
-  </si>
-  <si>
     <t>Assassins</t>
   </si>
   <si>
@@ -467,9 +464,6 @@
     <t>Steven smith</t>
   </si>
   <si>
-    <t>Rahane</t>
-  </si>
-  <si>
     <t>Knockout</t>
   </si>
   <si>
@@ -797,9 +791,6 @@
     <t>Ravichandran Ashwin, Cheteshwar Pujara, Marnus Labuschagne</t>
   </si>
   <si>
-    <t>pujara</t>
-  </si>
-  <si>
     <t>nathan lyon</t>
   </si>
   <si>
@@ -854,9 +845,6 @@
     <t>Ravichandran Ashwin, Ravindra Jadeja, David Warner</t>
   </si>
   <si>
-    <t>Cummins</t>
-  </si>
-  <si>
     <t>Rohit Sharma, Marnus Labuschagne, David Warner</t>
   </si>
   <si>
@@ -873,6 +861,12 @@
   </si>
   <si>
     <t>Vice Captain</t>
+  </si>
+  <si>
+    <t>R Ashwin</t>
+  </si>
+  <si>
+    <t>Cheteshwar pujara</t>
   </si>
 </sst>
 </file>
@@ -1150,9 +1144,9 @@
   </sheetPr>
   <dimension ref="A1:L137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1188,19 +1182,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>6</v>
@@ -1276,7 +1270,7 @@
         <v>22</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>23</v>
+        <v>169</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>15</v>
@@ -1287,7 +1281,7 @@
         <v>44201.586965509261</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>9</v>
@@ -1302,22 +1296,22 @@
         <v>7455832515</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1325,34 +1319,34 @@
         <v>44201.691059675926</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="D5" s="5">
         <v>9548890016</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="4">
         <v>8755505991</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="K5" s="4" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>15</v>
@@ -1363,37 +1357,37 @@
         <v>44201.879794386579</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="F6" s="4">
         <v>9871507785</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1401,34 +1395,34 @@
         <v>44201.98132525463</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7" s="5">
         <v>9871215302</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F7" s="4">
         <v>9716207786</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>15</v>
@@ -1439,34 +1433,34 @@
         <v>44201.983994710652</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" s="5">
         <v>9716207786</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F8" s="4">
         <v>9871215303</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>15</v>
@@ -1477,34 +1471,34 @@
         <v>44202.218708530098</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" s="5">
         <v>9971238827</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F9" s="4">
         <v>852801729</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>15</v>
@@ -1515,37 +1509,37 @@
         <v>44202.684185578706</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="F10" s="4">
         <v>7073080957</v>
       </c>
       <c r="G10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="L10" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1553,25 +1547,25 @@
         <v>44202.687026435189</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11" s="5">
         <v>7737713070</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F11" s="4">
         <v>8358020112</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>21</v>
@@ -1580,10 +1574,10 @@
         <v>14</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1591,37 +1585,37 @@
         <v>44202.68860238426</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="D12" s="5">
         <v>8358020112</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F12" s="4">
         <v>7737713070</v>
       </c>
       <c r="G12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="K12" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1629,34 +1623,34 @@
         <v>44202.69418958333</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D13" s="5">
         <v>7073080957</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F13" s="4">
         <v>8860491682</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>15</v>
@@ -1667,37 +1661,37 @@
         <v>44202.807372627314</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D14" s="5">
         <v>9873809204</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F14" s="4">
         <v>7986989297</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I14" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="J14" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>90</v>
-      </c>
       <c r="L14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1705,37 +1699,37 @@
         <v>44202.825784722227</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D15" s="5">
         <v>9599340767</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F15" s="4">
         <v>9953610004</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="J15" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="L15" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1743,37 +1737,37 @@
         <v>44202.845316215273</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="D16" s="5">
         <v>9953610004</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F16" s="4">
         <v>9599340767</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1781,34 +1775,34 @@
         <v>44202.874126828705</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D17" s="5">
         <v>9888185875</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F17" s="4">
         <v>9306139886</v>
       </c>
       <c r="G17" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="J17" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>15</v>
@@ -1819,37 +1813,37 @@
         <v>44202.886415937501</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D18" s="5">
         <v>2405211256</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F18" s="4">
         <v>2405799130</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1857,37 +1851,37 @@
         <v>44202.890595983801</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="D19" s="5">
         <v>2405799130</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F19" s="4">
         <v>2405211256</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>14</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1895,34 +1889,34 @@
         <v>44202.93270686343</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="D20" s="5">
         <v>9306139886</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F20" s="4">
         <v>9888185875</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>15</v>
@@ -1933,37 +1927,37 @@
         <v>44202.949469143517</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D21" s="5">
         <v>9829526588</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F21" s="4">
         <v>7907745747</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>14</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1971,25 +1965,25 @@
         <v>44202.962837106483</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D22" s="5">
         <v>8467891974</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F22" s="4">
         <v>9729380075</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>21</v>
@@ -1998,7 +1992,7 @@
         <v>14</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>15</v>
@@ -2009,34 +2003,34 @@
         <v>44202.965974062499</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D23" s="4">
         <v>9871826479</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F23" s="4">
         <v>9899046374</v>
       </c>
       <c r="G23" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>125</v>
-      </c>
       <c r="K23" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>15</v>
@@ -2047,31 +2041,31 @@
         <v>44202.965977071755</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="D24" s="4">
         <v>9899046374</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F24" s="4">
         <v>9871826479</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>12</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>14</v>
@@ -2085,37 +2079,37 @@
         <v>44202.968508217593</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>116</v>
       </c>
       <c r="D25" s="5">
         <v>7907745747</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F25" s="4">
         <v>9829526588</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>14</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2123,31 +2117,31 @@
         <v>44202.981191863422</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D26" s="4">
         <v>9650523994</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F26" s="4">
         <v>9899539075</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>22</v>
@@ -2161,34 +2155,34 @@
         <v>44202.98651239583</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="D27" s="5">
         <v>9899539075</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F27" s="4">
         <v>9650523994</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L27" s="4" t="s">
         <v>15</v>
@@ -2199,37 +2193,37 @@
         <v>44203.018112361111</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D28" s="4">
         <v>9654138482</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F28" s="4">
         <v>8287819109</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2237,37 +2231,37 @@
         <v>44203.01887190972</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="D29" s="4">
         <v>8287819109</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F29" s="4">
         <v>9654138482</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I29" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="J29" s="4" t="s">
-        <v>139</v>
-      </c>
       <c r="K29" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2275,37 +2269,37 @@
         <v>44203.082408368056</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D30" s="4">
         <v>9871507785</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="H30" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I30" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="J30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="K30" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="L30" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="L30" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2313,37 +2307,37 @@
         <v>44203.194539814816</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D31" s="5">
         <v>7986989297</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F31" s="4">
         <v>9873809204</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>21</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2351,34 +2345,34 @@
         <v>44203.198197106482</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D32" s="5">
         <v>8950100272</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F32" s="4">
         <v>9996391888</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L32" s="4" t="s">
         <v>15</v>
@@ -2389,34 +2383,34 @@
         <v>44203.199115555559</v>
       </c>
       <c r="B33" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="H33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>159</v>
-      </c>
       <c r="J33" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>15</v>
@@ -2427,34 +2421,34 @@
         <v>44203.201179826385</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D34" s="5">
         <v>9996391888</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F34" s="4">
         <v>8950100272</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>15</v>
@@ -2465,34 +2459,34 @@
         <v>44203.201208483792</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I35" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J35" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J35" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="K35" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L35" s="4" t="s">
         <v>15</v>
@@ -2503,34 +2497,34 @@
         <v>44203.201836875</v>
       </c>
       <c r="B36" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>119</v>
       </c>
       <c r="D36" s="5">
         <v>9729380075</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F36" s="4">
         <v>8467891972</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>166</v>
+        <v>69</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>23</v>
+        <v>169</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>15</v>
@@ -2541,34 +2535,34 @@
         <v>44203.206648900465</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="D37" s="5">
         <v>852801729</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F37" s="4">
         <v>9971238827</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L37" s="4" t="s">
         <v>15</v>

</xml_diff>